<commit_message>
change font size with ctrl+mouse wheel
</commit_message>
<xml_diff>
--- a/IDE-todo.xlsx
+++ b/IDE-todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>具体功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,10 +84,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>语法高亮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>代码折叠</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -228,15 +224,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>外部文件编辑变化监控</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Linux支持</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MacOS支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(简单的)语法高亮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分割布局支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单文件查找/替换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多文件查找</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找替换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正则表达式支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>括号匹配显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选中词高亮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动缩进</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>符号自动补全/覆盖</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -586,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -678,185 +710,223 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
+      <c r="B18" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>42</v>
-      </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>51</v>
+      <c r="B44" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>